<commit_message>
Remove fitness New caps
</commit_message>
<xml_diff>
--- a/server/data/allgamesnardin_24.xlsx
+++ b/server/data/allgamesnardin_24.xlsx
@@ -108,12 +108,12 @@
     <t xml:space="preserve">23*</t>
   </si>
   <si>
+    <t xml:space="preserve">Rugby Club Winterthur 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Albaladejo Rugby Club Lausanne 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Rugby Club Winterthur 1</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ligue C</t>
   </si>
   <si>
@@ -279,12 +279,12 @@
     <t xml:space="preserve">Lenggenhager Louie-Alan</t>
   </si>
   <si>
+    <t xml:space="preserve">Rugby Club Winterthur 2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Albaladejo Rugby Club Lausanne 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Rugby Club Winterthur 2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Ligue D</t>
   </si>
   <si>
@@ -360,10 +360,10 @@
     <t xml:space="preserve">Loehrer Rolf</t>
   </si>
   <si>
+    <t xml:space="preserve">Winterthur Ladies</t>
+  </si>
+  <si>
     <t xml:space="preserve">Basel Birds 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Winterthur Ladies</t>
   </si>
   <si>
     <t xml:space="preserve">Championnat Feminin, Ligue B</t>
@@ -7427,8 +7427,8 @@
   </sheetPr>
   <dimension ref="A1:AX370"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X51" activeCellId="0" sqref="X51"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A343" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B343" activeCellId="0" sqref="B343"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7905,10 +7905,10 @@
       <c r="A6" s="11" t="n">
         <v>45248</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="8" t="s">
         <v>85</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -7921,10 +7921,10 @@
         <v>40810</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>87</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="D7" s="15" t="s">
         <v>29</v>
@@ -7996,10 +7996,10 @@
         <v>41195</v>
       </c>
       <c r="B8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>87</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>29</v>
@@ -8073,10 +8073,10 @@
         <v>40110</v>
       </c>
       <c r="B9" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>86</v>
@@ -8142,10 +8142,10 @@
         <v>40670</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>97</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>86</v>
@@ -8218,10 +8218,10 @@
       <c r="A11" s="11" t="n">
         <v>43554</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="10" t="s">
         <v>112</v>
       </c>
       <c r="D11" s="10" t="s">
@@ -8348,11 +8348,11 @@
       <c r="A13" s="11" t="n">
         <v>44849</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>137</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>86</v>
@@ -8408,10 +8408,10 @@
         <v>43211</v>
       </c>
       <c r="B14" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>146</v>
@@ -8477,10 +8477,10 @@
         <v>44660</v>
       </c>
       <c r="B15" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>86</v>
@@ -8560,10 +8560,10 @@
         <v>44730</v>
       </c>
       <c r="B16" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>86</v>
@@ -8635,10 +8635,10 @@
         <v>45031</v>
       </c>
       <c r="B17" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>86</v>
@@ -8713,11 +8713,11 @@
       <c r="A18" s="11" t="n">
         <v>45416</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>155</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>85</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>86</v>
@@ -8785,10 +8785,10 @@
         <v>43029</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>176</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>146</v>
@@ -8855,11 +8855,11 @@
       <c r="A20" s="11" t="n">
         <v>43372</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>181</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>113</v>
@@ -8918,11 +8918,11 @@
       <c r="A21" s="11" t="n">
         <v>43729</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>181</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>113</v>
@@ -8979,11 +8979,11 @@
       <c r="A22" s="11" t="n">
         <v>44358</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>181</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>113</v>
@@ -9016,11 +9016,11 @@
       <c r="A23" s="11" t="n">
         <v>44450</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>181</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>113</v>
@@ -9053,11 +9053,11 @@
       <c r="A24" s="11" t="n">
         <v>45031</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>181</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>113</v>
@@ -9116,11 +9116,11 @@
       <c r="A25" s="11" t="n">
         <v>45213</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>181</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>113</v>
@@ -9153,11 +9153,11 @@
       <c r="A26" s="11" t="n">
         <v>45220</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>181</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>113</v>
@@ -9213,10 +9213,10 @@
         <v>45402</v>
       </c>
       <c r="B27" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>181</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>113</v>
@@ -9265,11 +9265,11 @@
       <c r="A28" s="11" t="n">
         <v>44632</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>187</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>188</v>
@@ -9341,10 +9341,10 @@
         <v>40097</v>
       </c>
       <c r="B29" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" s="8" t="s">
         <v>191</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>86</v>
@@ -9410,10 +9410,10 @@
         <v>40629</v>
       </c>
       <c r="B30" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>191</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>86</v>
@@ -9491,10 +9491,10 @@
         <v>43184</v>
       </c>
       <c r="B31" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>198</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>146</v>
@@ -9562,10 +9562,10 @@
         <v>43596</v>
       </c>
       <c r="B32" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>200</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>113</v>
@@ -9626,11 +9626,11 @@
       <c r="A33" s="11" t="n">
         <v>45220</v>
       </c>
-      <c r="B33" s="16" t="s">
+      <c r="B33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="16" t="s">
         <v>201</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>52</v>
@@ -9701,11 +9701,11 @@
       <c r="A34" s="11" t="n">
         <v>45220</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C34" s="16" t="s">
         <v>203</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>86</v>
@@ -9771,10 +9771,10 @@
         <v>42260</v>
       </c>
       <c r="B35" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>206</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>86</v>
@@ -9848,10 +9848,10 @@
         <v>43043</v>
       </c>
       <c r="B36" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>215</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>146</v>
@@ -9917,10 +9917,10 @@
         <v>44849</v>
       </c>
       <c r="B37" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>215</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>113</v>
@@ -9976,10 +9976,10 @@
         <v>45220</v>
       </c>
       <c r="B38" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>215</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>113</v>
@@ -10034,11 +10034,11 @@
       <c r="A39" s="11" t="n">
         <v>45227</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="10" t="s">
         <v>215</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>113</v>
@@ -10072,10 +10072,10 @@
         <v>43008</v>
       </c>
       <c r="B40" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="8" t="s">
         <v>219</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>146</v>
@@ -10139,10 +10139,10 @@
         <v>41531</v>
       </c>
       <c r="B41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>223</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D41" s="10" t="s">
         <v>52</v>
@@ -10214,10 +10214,10 @@
         <v>42119</v>
       </c>
       <c r="B42" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>223</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D42" s="10" t="s">
         <v>52</v>
@@ -10291,10 +10291,10 @@
         <v>42287</v>
       </c>
       <c r="B43" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>223</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D43" s="10" t="s">
         <v>52</v>
@@ -10372,10 +10372,10 @@
         <v>42651</v>
       </c>
       <c r="B44" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>223</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D44" s="10" t="s">
         <v>52</v>
@@ -10455,10 +10455,10 @@
         <v>43232</v>
       </c>
       <c r="B45" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>223</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D45" s="10" t="s">
         <v>52</v>
@@ -10537,11 +10537,11 @@
       <c r="A46" s="11" t="n">
         <v>45185</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B46" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="10" t="s">
         <v>223</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>52</v>
@@ -10614,11 +10614,11 @@
       <c r="A47" s="11" t="n">
         <v>42119</v>
       </c>
-      <c r="B47" s="8" t="s">
+      <c r="B47" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>238</v>
-      </c>
-      <c r="C47" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D47" s="10" t="s">
         <v>86</v>
@@ -10679,11 +10679,11 @@
       <c r="A48" s="11" t="n">
         <v>42287</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>238</v>
-      </c>
-      <c r="C48" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D48" s="10" t="s">
         <v>86</v>
@@ -10760,11 +10760,11 @@
       <c r="A49" s="11" t="n">
         <v>43232</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>238</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>85</v>
       </c>
       <c r="D49" s="10" t="s">
         <v>86</v>
@@ -10838,10 +10838,10 @@
         <v>40797</v>
       </c>
       <c r="B50" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>251</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D50" s="15" t="s">
         <v>29</v>
@@ -10919,10 +10919,10 @@
         <v>41525</v>
       </c>
       <c r="B51" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>251</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>52</v>
@@ -10996,10 +10996,10 @@
         <v>41910</v>
       </c>
       <c r="B52" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>251</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D52" s="10" t="s">
         <v>52</v>
@@ -11071,10 +11071,10 @@
         <v>41518</v>
       </c>
       <c r="B53" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>254</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D53" s="10" t="s">
         <v>52</v>
@@ -11152,10 +11152,10 @@
         <v>41895</v>
       </c>
       <c r="B54" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>254</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D54" s="10" t="s">
         <v>52</v>
@@ -11228,11 +11228,11 @@
       <c r="A55" s="11" t="n">
         <v>43401</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="B55" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="10" t="s">
         <v>254</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D55" s="10" t="s">
         <v>52</v>
@@ -11307,11 +11307,11 @@
       <c r="A56" s="11" t="n">
         <v>43716</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="B56" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="10" t="s">
         <v>254</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D56" s="10" t="s">
         <v>52</v>
@@ -11384,11 +11384,11 @@
       <c r="A57" s="11" t="n">
         <v>44087</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="B57" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="10" t="s">
         <v>254</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D57" s="10" t="s">
         <v>52</v>
@@ -11465,11 +11465,11 @@
       <c r="A58" s="11" t="n">
         <v>44451</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58" s="10" t="s">
         <v>254</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D58" s="10" t="s">
         <v>52</v>
@@ -11542,11 +11542,11 @@
       <c r="A59" s="11" t="n">
         <v>45059</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" s="10" t="s">
         <v>254</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D59" s="10" t="s">
         <v>52</v>
@@ -11624,10 +11624,10 @@
         <v>43596</v>
       </c>
       <c r="B60" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>264</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D60" s="10" t="s">
         <v>52</v>
@@ -11705,10 +11705,10 @@
         <v>43596</v>
       </c>
       <c r="B61" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>266</v>
-      </c>
-      <c r="C61" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D61" s="10" t="s">
         <v>86</v>
@@ -11778,10 +11778,10 @@
         <v>41538</v>
       </c>
       <c r="B62" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D62" s="10" t="s">
         <v>52</v>
@@ -11857,10 +11857,10 @@
         <v>42105</v>
       </c>
       <c r="B63" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C63" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="C63" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D63" s="10" t="s">
         <v>52</v>
@@ -11934,10 +11934,10 @@
         <v>42252</v>
       </c>
       <c r="B64" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C64" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="C64" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D64" s="10" t="s">
         <v>52</v>
@@ -12013,10 +12013,10 @@
         <v>42616</v>
       </c>
       <c r="B65" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C65" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="C65" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D65" s="10" t="s">
         <v>52</v>
@@ -12093,11 +12093,11 @@
       <c r="A66" s="11" t="n">
         <v>43204</v>
       </c>
-      <c r="B66" s="8" t="s">
+      <c r="B66" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C66" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="C66" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="D66" s="10" t="s">
         <v>52</v>
@@ -12176,11 +12176,11 @@
       <c r="A67" s="11" t="n">
         <v>43344</v>
       </c>
-      <c r="B67" s="8" t="s">
+      <c r="B67" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C67" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="C67" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="D67" s="10" t="s">
         <v>52</v>
@@ -12256,10 +12256,10 @@
         <v>40082</v>
       </c>
       <c r="B68" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C68" s="8" t="s">
         <v>274</v>
-      </c>
-      <c r="C68" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D68" s="10" t="s">
         <v>86</v>
@@ -12329,10 +12329,10 @@
         <v>40474</v>
       </c>
       <c r="B69" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C69" s="8" t="s">
         <v>274</v>
-      </c>
-      <c r="C69" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D69" s="10" t="s">
         <v>86</v>
@@ -12406,10 +12406,10 @@
         <v>42105</v>
       </c>
       <c r="B70" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C70" s="10" t="s">
         <v>274</v>
-      </c>
-      <c r="C70" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D70" s="10" t="s">
         <v>86</v>
@@ -12477,10 +12477,10 @@
         <v>42252</v>
       </c>
       <c r="B71" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C71" s="10" t="s">
         <v>274</v>
-      </c>
-      <c r="C71" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D71" s="10" t="s">
         <v>86</v>
@@ -12556,10 +12556,10 @@
         <v>42616</v>
       </c>
       <c r="B72" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C72" s="8" t="s">
         <v>274</v>
-      </c>
-      <c r="C72" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D72" s="10" t="s">
         <v>278</v>
@@ -12632,11 +12632,11 @@
       <c r="A73" s="11" t="n">
         <v>43204</v>
       </c>
-      <c r="B73" s="8" t="s">
+      <c r="B73" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C73" s="8" t="s">
         <v>274</v>
-      </c>
-      <c r="C73" s="12" t="s">
-        <v>85</v>
       </c>
       <c r="D73" s="10" t="s">
         <v>86</v>
@@ -12706,10 +12706,10 @@
         <v>41889</v>
       </c>
       <c r="B74" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C74" s="10" t="s">
         <v>281</v>
-      </c>
-      <c r="C74" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D74" s="10" t="s">
         <v>86</v>
@@ -12787,10 +12787,10 @@
         <v>42525</v>
       </c>
       <c r="B75" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C75" s="10" t="s">
         <v>281</v>
-      </c>
-      <c r="C75" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D75" s="10" t="s">
         <v>86</v>
@@ -12864,10 +12864,10 @@
         <v>43366</v>
       </c>
       <c r="B76" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C76" s="8" t="s">
         <v>281</v>
-      </c>
-      <c r="C76" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D76" s="10" t="s">
         <v>86</v>
@@ -12937,10 +12937,10 @@
         <v>45066</v>
       </c>
       <c r="B77" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C77" s="8" t="s">
         <v>281</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D77" s="10" t="s">
         <v>86</v>
@@ -13005,11 +13005,11 @@
       <c r="A78" s="11" t="n">
         <v>42483</v>
       </c>
-      <c r="B78" s="16" t="s">
+      <c r="B78" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C78" s="16" t="s">
         <v>293</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D78" s="10" t="s">
         <v>52</v>
@@ -13084,11 +13084,11 @@
       <c r="A79" s="11" t="n">
         <v>42483</v>
       </c>
-      <c r="B79" s="8" t="s">
+      <c r="B79" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C79" s="8" t="s">
         <v>294</v>
-      </c>
-      <c r="C79" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D79" s="10" t="s">
         <v>86</v>
@@ -13160,10 +13160,10 @@
         <v>40089</v>
       </c>
       <c r="B80" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C80" s="8" t="s">
         <v>296</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D80" s="10" t="s">
         <v>86</v>
@@ -13239,10 +13239,10 @@
         <v>40677</v>
       </c>
       <c r="B81" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C81" s="8" t="s">
         <v>296</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D81" s="10" t="s">
         <v>86</v>
@@ -13318,10 +13318,10 @@
         <v>41762</v>
       </c>
       <c r="B82" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C82" s="8" t="s">
         <v>300</v>
-      </c>
-      <c r="C82" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D82" s="10" t="s">
         <v>52</v>
@@ -13393,10 +13393,10 @@
         <v>41902</v>
       </c>
       <c r="B83" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C83" s="8" t="s">
         <v>300</v>
-      </c>
-      <c r="C83" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D83" s="10" t="s">
         <v>52</v>
@@ -13472,10 +13472,10 @@
         <v>43351</v>
       </c>
       <c r="B84" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>300</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D84" s="10" t="s">
         <v>52</v>
@@ -13553,10 +13553,10 @@
         <v>44681</v>
       </c>
       <c r="B85" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C85" s="8" t="s">
         <v>300</v>
-      </c>
-      <c r="C85" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D85" s="10" t="s">
         <v>52</v>
@@ -13634,10 +13634,10 @@
         <v>45017</v>
       </c>
       <c r="B86" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C86" s="8" t="s">
         <v>300</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D86" s="10" t="s">
         <v>52</v>
@@ -13711,10 +13711,10 @@
         <v>45199</v>
       </c>
       <c r="B87" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C87" s="8" t="s">
         <v>300</v>
-      </c>
-      <c r="C87" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D87" s="10" t="s">
         <v>52</v>
@@ -13788,10 +13788,10 @@
         <v>41755</v>
       </c>
       <c r="B88" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C88" s="8" t="s">
         <v>302</v>
-      </c>
-      <c r="C88" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D88" s="10" t="s">
         <v>52</v>
@@ -13867,10 +13867,10 @@
         <v>42154</v>
       </c>
       <c r="B89" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C89" s="8" t="s">
         <v>302</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D89" s="10" t="s">
         <v>52</v>
@@ -13944,10 +13944,10 @@
         <v>42847</v>
       </c>
       <c r="B90" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C90" s="8" t="s">
         <v>302</v>
-      </c>
-      <c r="C90" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D90" s="10" t="s">
         <v>52</v>
@@ -14019,10 +14019,10 @@
         <v>43603</v>
       </c>
       <c r="B91" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C91" s="8" t="s">
         <v>302</v>
-      </c>
-      <c r="C91" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D91" s="10" t="s">
         <v>52</v>
@@ -14088,10 +14088,10 @@
         <v>43729</v>
       </c>
       <c r="B92" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C92" s="8" t="s">
         <v>302</v>
-      </c>
-      <c r="C92" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D92" s="10" t="s">
         <v>52</v>
@@ -14167,10 +14167,10 @@
         <v>44492</v>
       </c>
       <c r="B93" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C93" s="8" t="s">
         <v>302</v>
-      </c>
-      <c r="C93" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D93" s="10" t="s">
         <v>52</v>
@@ -14242,10 +14242,10 @@
         <v>44814</v>
       </c>
       <c r="B94" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C94" s="8" t="s">
         <v>302</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D94" s="10" t="s">
         <v>52</v>
@@ -14315,10 +14315,10 @@
         <v>45444</v>
       </c>
       <c r="B95" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C95" s="8" t="s">
         <v>302</v>
-      </c>
-      <c r="C95" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D95" s="10" t="s">
         <v>52</v>
@@ -14395,11 +14395,11 @@
       <c r="A96" s="11" t="n">
         <v>42798</v>
       </c>
-      <c r="B96" s="16" t="s">
+      <c r="B96" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C96" s="16" t="s">
         <v>308</v>
-      </c>
-      <c r="C96" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D96" s="10" t="s">
         <v>52</v>
@@ -14476,11 +14476,11 @@
       <c r="A97" s="11" t="n">
         <v>42995</v>
       </c>
-      <c r="B97" s="16" t="s">
+      <c r="B97" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C97" s="16" t="s">
         <v>308</v>
-      </c>
-      <c r="C97" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D97" s="10" t="s">
         <v>52</v>
@@ -14559,11 +14559,11 @@
       <c r="A98" s="11" t="n">
         <v>43415</v>
       </c>
-      <c r="B98" s="16" t="s">
+      <c r="B98" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C98" s="16" t="s">
         <v>308</v>
-      </c>
-      <c r="C98" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D98" s="10" t="s">
         <v>52</v>
@@ -14642,11 +14642,11 @@
       <c r="A99" s="11" t="n">
         <v>44500</v>
       </c>
-      <c r="B99" s="16" t="s">
+      <c r="B99" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C99" s="16" t="s">
         <v>308</v>
-      </c>
-      <c r="C99" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D99" s="10" t="s">
         <v>52</v>
@@ -14723,11 +14723,11 @@
       <c r="A100" s="11" t="n">
         <v>44822</v>
       </c>
-      <c r="B100" s="16" t="s">
+      <c r="B100" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C100" s="16" t="s">
         <v>308</v>
-      </c>
-      <c r="C100" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D100" s="10" t="s">
         <v>52</v>
@@ -14801,10 +14801,10 @@
         <v>40061</v>
       </c>
       <c r="B101" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C101" s="8" t="s">
         <v>310</v>
-      </c>
-      <c r="C101" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D101" s="10" t="s">
         <v>86</v>
@@ -14871,11 +14871,11 @@
       <c r="A102" s="11" t="n">
         <v>41917</v>
       </c>
-      <c r="B102" s="8" t="s">
+      <c r="B102" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C102" s="8" t="s">
         <v>310</v>
-      </c>
-      <c r="C102" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D102" s="10" t="s">
         <v>86</v>
@@ -14940,11 +14940,11 @@
       <c r="A103" s="11" t="n">
         <v>42441</v>
       </c>
-      <c r="B103" s="8" t="s">
+      <c r="B103" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C103" s="8" t="s">
         <v>310</v>
-      </c>
-      <c r="C103" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D103" s="10" t="s">
         <v>86</v>
@@ -14978,10 +14978,10 @@
         <v>44822</v>
       </c>
       <c r="B104" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C104" s="8" t="s">
         <v>310</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D104" s="10" t="s">
         <v>86</v>
@@ -15037,10 +15037,10 @@
         <v>45052</v>
       </c>
       <c r="B105" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C105" s="10" t="s">
         <v>310</v>
-      </c>
-      <c r="C105" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D105" s="10" t="s">
         <v>86</v>
@@ -15098,10 +15098,10 @@
         <v>41580</v>
       </c>
       <c r="B106" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C106" s="8" t="s">
         <v>313</v>
-      </c>
-      <c r="C106" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D106" s="10" t="s">
         <v>52</v>
@@ -15175,10 +15175,10 @@
         <v>41881</v>
       </c>
       <c r="B107" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C107" s="8" t="s">
         <v>313</v>
-      </c>
-      <c r="C107" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D107" s="10" t="s">
         <v>52</v>
@@ -15256,10 +15256,10 @@
         <v>42861</v>
       </c>
       <c r="B108" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C108" s="8" t="s">
         <v>313</v>
-      </c>
-      <c r="C108" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D108" s="10" t="s">
         <v>52</v>
@@ -15336,11 +15336,11 @@
       <c r="A109" s="11" t="n">
         <v>44891</v>
       </c>
-      <c r="B109" s="8" t="s">
+      <c r="B109" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C109" s="8" t="s">
         <v>313</v>
-      </c>
-      <c r="C109" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D109" s="10" t="s">
         <v>188</v>
@@ -15373,11 +15373,11 @@
       <c r="A110" s="11" t="n">
         <v>41881</v>
       </c>
-      <c r="B110" s="8" t="s">
+      <c r="B110" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C110" s="8" t="s">
         <v>314</v>
-      </c>
-      <c r="C110" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D110" s="10" t="s">
         <v>86</v>
@@ -15410,11 +15410,11 @@
       <c r="A111" s="11" t="n">
         <v>43715</v>
       </c>
-      <c r="B111" s="8" t="s">
+      <c r="B111" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C111" s="8" t="s">
         <v>315</v>
-      </c>
-      <c r="C111" s="12" t="s">
-        <v>85</v>
       </c>
       <c r="D111" s="10" t="s">
         <v>86</v>
@@ -15478,10 +15478,10 @@
         <v>44450</v>
       </c>
       <c r="B112" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C112" s="10" t="s">
         <v>317</v>
-      </c>
-      <c r="C112" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D112" s="10" t="s">
         <v>86</v>
@@ -15553,10 +15553,10 @@
         <v>44702</v>
       </c>
       <c r="B113" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C113" s="8" t="s">
         <v>321</v>
-      </c>
-      <c r="C113" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D113" s="10" t="s">
         <v>86</v>
@@ -15590,10 +15590,10 @@
         <v>40642</v>
       </c>
       <c r="B114" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C114" s="8" t="s">
         <v>322</v>
-      </c>
-      <c r="C114" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D114" s="10" t="s">
         <v>86</v>
@@ -15671,10 +15671,10 @@
         <v>41391</v>
       </c>
       <c r="B115" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C115" s="12" t="s">
         <v>322</v>
-      </c>
-      <c r="C115" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="D115" s="9" t="s">
         <v>29</v>
@@ -15752,10 +15752,10 @@
         <v>40103</v>
       </c>
       <c r="B116" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C116" s="8" t="s">
         <v>324</v>
-      </c>
-      <c r="C116" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D116" s="10" t="s">
         <v>86</v>
@@ -15815,10 +15815,10 @@
         <v>40649</v>
       </c>
       <c r="B117" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C117" s="8" t="s">
         <v>324</v>
-      </c>
-      <c r="C117" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D117" s="10" t="s">
         <v>86</v>
@@ -15892,10 +15892,10 @@
         <v>40824</v>
       </c>
       <c r="B118" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C118" s="14" t="s">
         <v>324</v>
-      </c>
-      <c r="C118" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="D118" s="15" t="s">
         <v>29</v>
@@ -15973,10 +15973,10 @@
         <v>41181</v>
       </c>
       <c r="B119" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C119" s="12" t="s">
         <v>324</v>
-      </c>
-      <c r="C119" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="D119" s="9" t="s">
         <v>29</v>
@@ -16053,11 +16053,11 @@
       <c r="A120" s="11" t="n">
         <v>44499</v>
       </c>
-      <c r="B120" s="12" t="s">
+      <c r="B120" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C120" s="12" t="s">
         <v>324</v>
-      </c>
-      <c r="C120" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D120" s="10" t="s">
         <v>86</v>
@@ -16125,7 +16125,7 @@
         <v>40117</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C121" s="8" t="s">
         <v>324</v>
@@ -16257,7 +16257,7 @@
         <v>40124</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C122" s="8" t="s">
         <v>342</v>
@@ -16317,7 +16317,7 @@
         <v>40264</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C123" s="8" t="s">
         <v>274</v>
@@ -16451,7 +16451,7 @@
         <v>40278</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C124" s="8" t="s">
         <v>296</v>
@@ -16589,7 +16589,7 @@
         <v>40292</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C125" s="8" t="s">
         <v>191</v>
@@ -16733,7 +16733,7 @@
         <v>40320</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C126" s="8" t="s">
         <v>310</v>
@@ -16793,7 +16793,7 @@
         <v>40342</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C127" s="8" t="s">
         <v>97</v>
@@ -16907,7 +16907,7 @@
         <v>40432</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C128" s="8" t="s">
         <v>296</v>
@@ -17041,7 +17041,7 @@
         <v>40446</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C129" s="8" t="s">
         <v>191</v>
@@ -17181,7 +17181,7 @@
         <v>40467</v>
       </c>
       <c r="B130" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C130" s="16" t="s">
         <v>324</v>
@@ -17321,7 +17321,7 @@
         <v>40481</v>
       </c>
       <c r="B131" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C131" s="8" t="s">
         <v>438</v>
@@ -17467,7 +17467,7 @@
         <v>40489</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C132" s="8" t="s">
         <v>97</v>
@@ -17585,7 +17585,7 @@
         <v>40621</v>
       </c>
       <c r="B133" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C133" s="16" t="s">
         <v>322</v>
@@ -17729,7 +17729,7 @@
         <v>40663</v>
       </c>
       <c r="B134" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C134" s="16" t="s">
         <v>274</v>
@@ -17865,7 +17865,7 @@
         <v>40817</v>
       </c>
       <c r="B135" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C135" s="14" t="s">
         <v>498</v>
@@ -18001,7 +18001,7 @@
         <v>40831</v>
       </c>
       <c r="B136" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C136" s="14" t="s">
         <v>515</v>
@@ -18133,7 +18133,7 @@
         <v>40838</v>
       </c>
       <c r="B137" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C137" s="18" t="s">
         <v>531</v>
@@ -18281,7 +18281,7 @@
         <v>40845</v>
       </c>
       <c r="B138" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C138" s="14" t="s">
         <v>251</v>
@@ -18429,7 +18429,7 @@
         <v>40999</v>
       </c>
       <c r="B139" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C139" s="16" t="s">
         <v>87</v>
@@ -18577,7 +18577,7 @@
         <v>41020</v>
       </c>
       <c r="B140" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C140" s="14" t="s">
         <v>324</v>
@@ -18719,7 +18719,7 @@
         <v>41041</v>
       </c>
       <c r="B141" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C141" s="14" t="s">
         <v>605</v>
@@ -18867,7 +18867,7 @@
         <v>41188</v>
       </c>
       <c r="B142" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C142" s="19" t="s">
         <v>322</v>
@@ -18927,10 +18927,10 @@
         <v>41202</v>
       </c>
       <c r="B143" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C143" s="12" t="s">
         <v>28</v>
-      </c>
-      <c r="C143" s="12" t="s">
-        <v>27</v>
       </c>
       <c r="D143" s="9" t="s">
         <v>29</v>
@@ -19063,7 +19063,7 @@
         <v>41223</v>
       </c>
       <c r="B144" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C144" s="12" t="s">
         <v>605</v>
@@ -19205,7 +19205,7 @@
         <v>41356</v>
       </c>
       <c r="B145" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C145" s="12" t="s">
         <v>515</v>
@@ -19349,7 +19349,7 @@
         <v>41371</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C146" s="8" t="s">
         <v>254</v>
@@ -19497,7 +19497,7 @@
         <v>41398</v>
       </c>
       <c r="B147" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C147" s="16" t="s">
         <v>87</v>
@@ -19557,7 +19557,7 @@
         <v>41419</v>
       </c>
       <c r="B148" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C148" s="12" t="s">
         <v>692</v>
@@ -19691,7 +19691,7 @@
         <v>41427</v>
       </c>
       <c r="B149" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C149" s="12" t="s">
         <v>324</v>
@@ -19825,7 +19825,7 @@
         <v>41461</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C150" s="8" t="s">
         <v>531</v>
@@ -19973,7 +19973,7 @@
         <v>41546</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C151" s="8" t="s">
         <v>720</v>
@@ -20115,10 +20115,10 @@
         <v>41559</v>
       </c>
       <c r="B152" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C152" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="C152" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="D152" s="10" t="s">
         <v>52</v>
@@ -20249,7 +20249,7 @@
         <v>41566</v>
       </c>
       <c r="B153" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C153" s="8" t="s">
         <v>302</v>
@@ -20381,7 +20381,7 @@
         <v>41573</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C154" s="8" t="s">
         <v>300</v>
@@ -20519,7 +20519,7 @@
         <v>41594</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C155" s="8" t="s">
         <v>223</v>
@@ -20653,7 +20653,7 @@
         <v>41713</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C156" s="8" t="s">
         <v>251</v>
@@ -20789,7 +20789,7 @@
         <v>41720</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C157" s="8" t="s">
         <v>270</v>
@@ -20935,7 +20935,7 @@
         <v>41734</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C158" s="8" t="s">
         <v>254</v>
@@ -21071,7 +21071,7 @@
         <v>41769</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C159" s="8" t="s">
         <v>313</v>
@@ -21219,7 +21219,7 @@
         <v>41777</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C160" s="8" t="s">
         <v>293</v>
@@ -21363,7 +21363,7 @@
         <v>41916</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C161" s="8" t="s">
         <v>881</v>
@@ -21507,7 +21507,7 @@
         <v>41923</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C162" s="8" t="s">
         <v>270</v>
@@ -21653,7 +21653,7 @@
         <v>41930</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C163" s="8" t="s">
         <v>223</v>
@@ -21797,7 +21797,7 @@
         <v>41937</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C164" s="8" t="s">
         <v>531</v>
@@ -21943,7 +21943,7 @@
         <v>41951</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C165" s="8" t="s">
         <v>302</v>
@@ -22079,7 +22079,7 @@
         <v>41958</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C166" s="8" t="s">
         <v>254</v>
@@ -22215,7 +22215,7 @@
         <v>42077</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C167" s="8" t="s">
         <v>313</v>
@@ -22363,7 +22363,7 @@
         <v>42084</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C168" s="8" t="s">
         <v>300</v>
@@ -22511,7 +22511,7 @@
         <v>42091</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C169" s="8" t="s">
         <v>251</v>
@@ -22639,7 +22639,7 @@
         <v>42294</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C170" s="8" t="s">
         <v>293</v>
@@ -22781,7 +22781,7 @@
         <v>42308</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C171" s="8" t="s">
         <v>270</v>
@@ -22929,7 +22929,7 @@
         <v>42315</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C172" s="8" t="s">
         <v>531</v>
@@ -23077,7 +23077,7 @@
         <v>42441</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C173" s="8" t="s">
         <v>1017</v>
@@ -23225,7 +23225,7 @@
         <v>42448</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C174" s="8" t="s">
         <v>223</v>
@@ -23371,7 +23371,7 @@
         <v>42490</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C175" s="8" t="s">
         <v>254</v>
@@ -23517,7 +23517,7 @@
         <v>42498</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C176" s="8" t="s">
         <v>251</v>
@@ -23653,7 +23653,7 @@
         <v>42511</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C177" s="8" t="s">
         <v>438</v>
@@ -23791,7 +23791,7 @@
         <v>42658</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C178" s="8" t="s">
         <v>308</v>
@@ -23935,7 +23935,7 @@
         <v>42672</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C179" s="8" t="s">
         <v>270</v>
@@ -24079,7 +24079,7 @@
         <v>42686</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C180" s="8" t="s">
         <v>692</v>
@@ -24219,7 +24219,7 @@
         <v>42812</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C181" s="8" t="s">
         <v>1017</v>
@@ -24369,7 +24369,7 @@
         <v>42826</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C182" s="8" t="s">
         <v>223</v>
@@ -24519,7 +24519,7 @@
         <v>42854</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C183" s="8" t="s">
         <v>270</v>
@@ -24669,7 +24669,7 @@
         <v>42875</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C184" s="8" t="s">
         <v>438</v>
@@ -24815,7 +24815,7 @@
         <v>42883</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C185" s="8" t="s">
         <v>692</v>
@@ -24963,7 +24963,7 @@
         <v>43015</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C186" s="8" t="s">
         <v>438</v>
@@ -25109,7 +25109,7 @@
         <v>43022</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C187" s="8" t="s">
         <v>270</v>
@@ -25259,7 +25259,7 @@
         <v>43197</v>
       </c>
       <c r="B188" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C188" s="8" t="s">
         <v>720</v>
@@ -25387,7 +25387,7 @@
         <v>43212</v>
       </c>
       <c r="B189" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C189" s="8" t="s">
         <v>223</v>
@@ -25537,7 +25537,7 @@
         <v>43225</v>
       </c>
       <c r="B190" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C190" s="8" t="s">
         <v>1017</v>
@@ -25677,7 +25677,7 @@
         <v>43236</v>
       </c>
       <c r="B191" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C191" s="8" t="s">
         <v>438</v>
@@ -25823,7 +25823,7 @@
         <v>43246</v>
       </c>
       <c r="B192" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C192" s="8" t="s">
         <v>270</v>
@@ -25973,7 +25973,7 @@
         <v>43365</v>
       </c>
       <c r="B193" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C193" s="8" t="s">
         <v>302</v>
@@ -26109,7 +26109,7 @@
         <v>43379</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C194" s="8" t="s">
         <v>438</v>
@@ -26257,7 +26257,7 @@
         <v>43394</v>
       </c>
       <c r="B195" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C195" s="8" t="s">
         <v>264</v>
@@ -26407,7 +26407,7 @@
         <v>43408</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C196" s="8" t="s">
         <v>270</v>
@@ -26541,7 +26541,7 @@
         <v>43554</v>
       </c>
       <c r="B197" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C197" s="8" t="s">
         <v>300</v>
@@ -26681,7 +26681,7 @@
         <v>43582</v>
       </c>
       <c r="B198" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C198" s="8" t="s">
         <v>308</v>
@@ -26819,7 +26819,7 @@
         <v>43610</v>
       </c>
       <c r="B199" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C199" s="8" t="s">
         <v>254</v>
@@ -26955,7 +26955,7 @@
         <v>43722</v>
       </c>
       <c r="B200" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C200" s="8" t="s">
         <v>293</v>
@@ -27095,7 +27095,7 @@
         <v>43743</v>
       </c>
       <c r="B201" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C201" s="8" t="s">
         <v>300</v>
@@ -27241,7 +27241,7 @@
         <v>43771</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C202" s="8" t="s">
         <v>438</v>
@@ -27389,7 +27389,7 @@
         <v>44115</v>
       </c>
       <c r="B203" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C203" s="8" t="s">
         <v>300</v>
@@ -27535,7 +27535,7 @@
         <v>44478</v>
       </c>
       <c r="B204" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C204" s="8" t="s">
         <v>300</v>
@@ -27671,7 +27671,7 @@
         <v>44506</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C205" s="8" t="s">
         <v>438</v>
@@ -27821,7 +27821,7 @@
         <v>44674</v>
       </c>
       <c r="B206" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C206" s="8" t="s">
         <v>302</v>
@@ -27959,7 +27959,7 @@
         <v>44696</v>
       </c>
       <c r="B207" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C207" s="8" t="s">
         <v>1017</v>
@@ -28099,7 +28099,7 @@
         <v>44702</v>
       </c>
       <c r="B208" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C208" s="8" t="s">
         <v>308</v>
@@ -28249,7 +28249,7 @@
         <v>44710</v>
       </c>
       <c r="B209" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C209" s="8" t="s">
         <v>254</v>
@@ -28385,7 +28385,7 @@
         <v>44842</v>
       </c>
       <c r="B210" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C210" s="8" t="s">
         <v>438</v>
@@ -28531,7 +28531,7 @@
         <v>44870</v>
       </c>
       <c r="B211" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C211" s="8" t="s">
         <v>254</v>
@@ -28665,7 +28665,7 @@
         <v>44878</v>
       </c>
       <c r="B212" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C212" s="8" t="s">
         <v>300</v>
@@ -28805,7 +28805,7 @@
         <v>45003</v>
       </c>
       <c r="B213" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C213" s="8" t="s">
         <v>302</v>
@@ -28947,10 +28947,10 @@
         <v>45038</v>
       </c>
       <c r="B214" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C214" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="C214" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="D214" s="10" t="s">
         <v>52</v>
@@ -29095,7 +29095,7 @@
         <v>45045</v>
       </c>
       <c r="B215" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C215" s="8" t="s">
         <v>1017</v>
@@ -29237,7 +29237,7 @@
         <v>45052</v>
       </c>
       <c r="B216" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C216" s="8" t="s">
         <v>308</v>
@@ -29385,7 +29385,7 @@
         <v>45178</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C217" s="8" t="s">
         <v>1017</v>
@@ -29525,7 +29525,7 @@
         <v>45206</v>
       </c>
       <c r="B218" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C218" s="8" t="s">
         <v>302</v>
@@ -29665,7 +29665,7 @@
         <v>45227</v>
       </c>
       <c r="B219" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C219" s="8" t="s">
         <v>438</v>
@@ -29815,7 +29815,7 @@
         <v>45367</v>
       </c>
       <c r="B220" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C220" s="8" t="s">
         <v>223</v>
@@ -29965,7 +29965,7 @@
         <v>45388</v>
       </c>
       <c r="B221" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C221" s="8" t="s">
         <v>300</v>
@@ -30109,7 +30109,7 @@
         <v>45409</v>
       </c>
       <c r="B222" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C222" s="8" t="s">
         <v>201</v>
@@ -30259,10 +30259,10 @@
         <v>45438</v>
       </c>
       <c r="B223" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C223" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="C223" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="D223" s="10" t="s">
         <v>52</v>
@@ -30407,7 +30407,7 @@
         <v>41909</v>
       </c>
       <c r="B224" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C224" s="10" t="s">
         <v>1489</v>
@@ -30467,7 +30467,7 @@
         <v>41923</v>
       </c>
       <c r="B225" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C225" s="10" t="s">
         <v>274</v>
@@ -30607,7 +30607,7 @@
         <v>41930</v>
       </c>
       <c r="B226" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C226" s="10" t="s">
         <v>238</v>
@@ -30743,7 +30743,7 @@
         <v>41937</v>
       </c>
       <c r="B227" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C227" s="10" t="s">
         <v>1506</v>
@@ -30873,7 +30873,7 @@
         <v>41958</v>
       </c>
       <c r="B228" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C228" s="10" t="s">
         <v>310</v>
@@ -31015,7 +31015,7 @@
         <v>42077</v>
       </c>
       <c r="B229" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C229" s="10" t="s">
         <v>314</v>
@@ -31075,7 +31075,7 @@
         <v>42133</v>
       </c>
       <c r="B230" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C230" s="10" t="s">
         <v>281</v>
@@ -31211,7 +31211,7 @@
         <v>42273</v>
       </c>
       <c r="B231" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C231" s="10" t="s">
         <v>1489</v>
@@ -31343,7 +31343,7 @@
         <v>42294</v>
       </c>
       <c r="B232" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C232" s="10" t="s">
         <v>294</v>
@@ -31469,7 +31469,7 @@
         <v>42308</v>
       </c>
       <c r="B233" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C233" s="10" t="s">
         <v>274</v>
@@ -31615,7 +31615,7 @@
         <v>42315</v>
       </c>
       <c r="B234" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C234" s="10" t="s">
         <v>206</v>
@@ -31753,7 +31753,7 @@
         <v>42448</v>
       </c>
       <c r="B235" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C235" s="10" t="s">
         <v>238</v>
@@ -31885,7 +31885,7 @@
         <v>42490</v>
       </c>
       <c r="B236" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C236" s="10" t="s">
         <v>310</v>
@@ -31945,7 +31945,7 @@
         <v>42498</v>
       </c>
       <c r="B237" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C237" s="10" t="s">
         <v>281</v>
@@ -32085,7 +32085,7 @@
         <v>42672</v>
       </c>
       <c r="B238" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C238" s="8" t="s">
         <v>274</v>
@@ -32225,7 +32225,7 @@
         <v>42686</v>
       </c>
       <c r="B239" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C239" s="8" t="s">
         <v>1489</v>
@@ -32285,7 +32285,7 @@
         <v>42812</v>
       </c>
       <c r="B240" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C240" s="12" t="s">
         <v>605</v>
@@ -32345,7 +32345,7 @@
         <v>42820</v>
       </c>
       <c r="B241" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C241" s="8" t="s">
         <v>187</v>
@@ -32495,7 +32495,7 @@
         <v>42826</v>
       </c>
       <c r="B242" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C242" s="8" t="s">
         <v>238</v>
@@ -32623,7 +32623,7 @@
         <v>42896</v>
       </c>
       <c r="B243" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C243" s="8" t="s">
         <v>187</v>
@@ -32769,7 +32769,7 @@
         <v>43022</v>
       </c>
       <c r="B244" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C244" s="8" t="s">
         <v>274</v>
@@ -32911,7 +32911,7 @@
         <v>43169</v>
       </c>
       <c r="B245" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C245" s="8" t="s">
         <v>1625</v>
@@ -33043,7 +33043,7 @@
         <v>43218</v>
       </c>
       <c r="B246" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C246" s="8" t="s">
         <v>1643</v>
@@ -33103,7 +33103,7 @@
         <v>43225</v>
       </c>
       <c r="B247" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C247" s="12" t="s">
         <v>605</v>
@@ -33237,7 +33237,7 @@
         <v>43246</v>
       </c>
       <c r="B248" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C248" s="8" t="s">
         <v>274</v>
@@ -33377,7 +33377,7 @@
         <v>43379</v>
       </c>
       <c r="B249" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C249" s="12" t="s">
         <v>605</v>
@@ -33523,7 +33523,7 @@
         <v>43400</v>
       </c>
       <c r="B250" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C250" s="12" t="s">
         <v>720</v>
@@ -33583,7 +33583,7 @@
         <v>43408</v>
       </c>
       <c r="B251" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C251" s="12" t="s">
         <v>281</v>
@@ -33723,10 +33723,10 @@
         <v>43428</v>
       </c>
       <c r="B252" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C252" s="10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D252" s="9" t="s">
         <v>188</v>
@@ -33857,7 +33857,7 @@
         <v>43562</v>
       </c>
       <c r="B253" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C253" s="12" t="s">
         <v>266</v>
@@ -33991,7 +33991,7 @@
         <v>43582</v>
       </c>
       <c r="B254" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C254" s="12" t="s">
         <v>1697</v>
@@ -34133,7 +34133,7 @@
         <v>43610</v>
       </c>
       <c r="B255" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C255" s="12" t="s">
         <v>1716</v>
@@ -34275,7 +34275,7 @@
         <v>43722</v>
       </c>
       <c r="B256" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C256" s="12" t="s">
         <v>281</v>
@@ -34403,7 +34403,7 @@
         <v>43743</v>
       </c>
       <c r="B257" s="12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C257" s="12" t="s">
         <v>1716</v>
@@ -34535,7 +34535,7 @@
         <v>44478</v>
       </c>
       <c r="B258" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C258" s="8" t="s">
         <v>1716</v>
@@ -34671,7 +34671,7 @@
         <v>44506</v>
       </c>
       <c r="B259" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C259" s="8" t="s">
         <v>155</v>
@@ -34819,7 +34819,7 @@
         <v>44674</v>
       </c>
       <c r="B260" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C260" s="8" t="s">
         <v>605</v>
@@ -34947,7 +34947,7 @@
         <v>44682</v>
       </c>
       <c r="B261" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C261" s="8" t="s">
         <v>324</v>
@@ -35083,7 +35083,7 @@
         <v>44724</v>
       </c>
       <c r="B262" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C262" s="8" t="s">
         <v>281</v>
@@ -35209,7 +35209,7 @@
         <v>44842</v>
       </c>
       <c r="B263" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C263" s="8" t="s">
         <v>155</v>
@@ -35343,7 +35343,7 @@
         <v>44870</v>
       </c>
       <c r="B264" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C264" s="8" t="s">
         <v>1697</v>
@@ -35485,7 +35485,7 @@
         <v>44878</v>
       </c>
       <c r="B265" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C265" s="8" t="s">
         <v>281</v>
@@ -35623,7 +35623,7 @@
         <v>45038</v>
       </c>
       <c r="B266" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C266" s="8" t="s">
         <v>137</v>
@@ -35759,7 +35759,7 @@
         <v>45045</v>
       </c>
       <c r="B267" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C267" s="8" t="s">
         <v>605</v>
@@ -35877,7 +35877,7 @@
         <v>45178</v>
       </c>
       <c r="B268" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C268" s="8" t="s">
         <v>605</v>
@@ -35999,7 +35999,7 @@
         <v>45227</v>
       </c>
       <c r="B269" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C269" s="8" t="s">
         <v>155</v>
@@ -36149,7 +36149,7 @@
         <v>45255</v>
       </c>
       <c r="B270" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C270" s="8" t="s">
         <v>251</v>
@@ -36209,7 +36209,7 @@
         <v>45409</v>
       </c>
       <c r="B271" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C271" s="8" t="s">
         <v>203</v>
@@ -36347,10 +36347,10 @@
         <v>45438</v>
       </c>
       <c r="B272" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C272" s="8" t="s">
         <v>85</v>
-      </c>
-      <c r="C272" s="8" t="s">
-        <v>84</v>
       </c>
       <c r="D272" s="10" t="s">
         <v>86</v>
@@ -36475,10 +36475,10 @@
         <v>41035</v>
       </c>
       <c r="B273" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C273" s="14" t="s">
         <v>531</v>
-      </c>
-      <c r="C273" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="D273" s="15" t="s">
         <v>29</v>
@@ -36556,10 +36556,10 @@
         <v>42169</v>
       </c>
       <c r="B274" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C274" s="8" t="s">
         <v>531</v>
-      </c>
-      <c r="C274" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D274" s="10" t="s">
         <v>52</v>
@@ -36633,10 +36633,10 @@
         <v>42259</v>
       </c>
       <c r="B275" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C275" s="8" t="s">
         <v>531</v>
-      </c>
-      <c r="C275" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D275" s="10" t="s">
         <v>52</v>
@@ -36711,11 +36711,11 @@
       <c r="A276" s="11" t="n">
         <v>42533</v>
       </c>
-      <c r="B276" s="8" t="s">
+      <c r="B276" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C276" s="8" t="s">
         <v>531</v>
-      </c>
-      <c r="C276" s="10" t="s">
-        <v>28</v>
       </c>
       <c r="D276" s="10" t="s">
         <v>52</v>
@@ -36793,10 +36793,10 @@
         <v>42169</v>
       </c>
       <c r="B277" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C277" s="10" t="s">
         <v>1506</v>
-      </c>
-      <c r="C277" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D277" s="10" t="s">
         <v>86</v>
@@ -36864,10 +36864,10 @@
         <v>41727</v>
       </c>
       <c r="B278" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C278" s="8" t="s">
         <v>720</v>
-      </c>
-      <c r="C278" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D278" s="10" t="s">
         <v>52</v>
@@ -36940,11 +36940,11 @@
       <c r="A279" s="11" t="n">
         <v>43253</v>
       </c>
-      <c r="B279" s="12" t="s">
+      <c r="B279" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C279" s="12" t="s">
         <v>720</v>
-      </c>
-      <c r="C279" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D279" s="10" t="s">
         <v>52</v>
@@ -37016,10 +37016,10 @@
         <v>43386</v>
       </c>
       <c r="B280" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C280" s="8" t="s">
         <v>720</v>
-      </c>
-      <c r="C280" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D280" s="10" t="s">
         <v>86</v>
@@ -37087,10 +37087,10 @@
         <v>41013</v>
       </c>
       <c r="B281" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C281" s="14" t="s">
         <v>498</v>
-      </c>
-      <c r="C281" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="D281" s="15" t="s">
         <v>29</v>
@@ -37168,10 +37168,10 @@
         <v>41209</v>
       </c>
       <c r="B282" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C282" s="12" t="s">
         <v>498</v>
-      </c>
-      <c r="C282" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="D282" s="9" t="s">
         <v>29</v>
@@ -37245,10 +37245,10 @@
         <v>41028</v>
       </c>
       <c r="B283" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C283" s="14" t="s">
         <v>515</v>
-      </c>
-      <c r="C283" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="D283" s="15" t="s">
         <v>29</v>
@@ -37324,10 +37324,10 @@
         <v>41175</v>
       </c>
       <c r="B284" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C284" s="12" t="s">
         <v>515</v>
-      </c>
-      <c r="C284" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="D284" s="9" t="s">
         <v>29</v>
@@ -37405,10 +37405,10 @@
         <v>40069</v>
       </c>
       <c r="B285" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C285" s="8" t="s">
         <v>342</v>
-      </c>
-      <c r="C285" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D285" s="10" t="s">
         <v>86</v>
@@ -37442,10 +37442,10 @@
         <v>42266</v>
       </c>
       <c r="B286" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C286" s="8" t="s">
         <v>1017</v>
-      </c>
-      <c r="C286" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D286" s="10" t="s">
         <v>52</v>
@@ -37519,10 +37519,10 @@
         <v>42665</v>
       </c>
       <c r="B287" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C287" s="8" t="s">
         <v>1017</v>
-      </c>
-      <c r="C287" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D287" s="10" t="s">
         <v>52</v>
@@ -37598,10 +37598,10 @@
         <v>43036</v>
       </c>
       <c r="B288" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C288" s="8" t="s">
         <v>1017</v>
-      </c>
-      <c r="C288" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D288" s="10" t="s">
         <v>52</v>
@@ -37680,11 +37680,11 @@
       <c r="A289" s="11" t="n">
         <v>43183</v>
       </c>
-      <c r="B289" s="8" t="s">
+      <c r="B289" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C289" s="8" t="s">
         <v>1017</v>
-      </c>
-      <c r="C289" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="D289" s="10" t="s">
         <v>52</v>
@@ -37763,11 +37763,11 @@
       <c r="A290" s="11" t="n">
         <v>43750</v>
       </c>
-      <c r="B290" s="8" t="s">
+      <c r="B290" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C290" s="8" t="s">
         <v>1017</v>
-      </c>
-      <c r="C290" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="D290" s="10" t="s">
         <v>52</v>
@@ -37840,11 +37840,11 @@
       <c r="A291" s="11" t="n">
         <v>44485</v>
       </c>
-      <c r="B291" s="8" t="s">
+      <c r="B291" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C291" s="8" t="s">
         <v>1017</v>
-      </c>
-      <c r="C291" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="D291" s="10" t="s">
         <v>52</v>
@@ -37923,11 +37923,11 @@
       <c r="A292" s="11" t="n">
         <v>44856</v>
       </c>
-      <c r="B292" s="8" t="s">
+      <c r="B292" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C292" s="8" t="s">
         <v>1017</v>
-      </c>
-      <c r="C292" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="D292" s="10" t="s">
         <v>52</v>
@@ -38002,11 +38002,11 @@
       <c r="A293" s="11" t="n">
         <v>45353</v>
       </c>
-      <c r="B293" s="8" t="s">
+      <c r="B293" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C293" s="8" t="s">
         <v>1017</v>
-      </c>
-      <c r="C293" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="D293" s="10" t="s">
         <v>52</v>
@@ -38084,10 +38084,10 @@
         <v>40852</v>
       </c>
       <c r="B294" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C294" s="14" t="s">
         <v>605</v>
-      </c>
-      <c r="C294" s="14" t="s">
-        <v>28</v>
       </c>
       <c r="D294" s="15" t="s">
         <v>29</v>
@@ -38165,10 +38165,10 @@
         <v>41167</v>
       </c>
       <c r="B295" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C295" s="12" t="s">
         <v>605</v>
-      </c>
-      <c r="C295" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="D295" s="9" t="s">
         <v>29</v>
@@ -38245,11 +38245,11 @@
       <c r="A296" s="11" t="n">
         <v>42665</v>
       </c>
-      <c r="B296" s="12" t="s">
+      <c r="B296" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C296" s="12" t="s">
         <v>605</v>
-      </c>
-      <c r="C296" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D296" s="10" t="s">
         <v>278</v>
@@ -38328,11 +38328,11 @@
       <c r="A297" s="11" t="n">
         <v>43036</v>
       </c>
-      <c r="B297" s="12" t="s">
+      <c r="B297" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C297" s="12" t="s">
         <v>605</v>
-      </c>
-      <c r="C297" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D297" s="10" t="s">
         <v>86</v>
@@ -38405,11 +38405,11 @@
       <c r="A298" s="11" t="n">
         <v>43183</v>
       </c>
-      <c r="B298" s="12" t="s">
+      <c r="B298" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C298" s="12" t="s">
         <v>605</v>
-      </c>
-      <c r="C298" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D298" s="10" t="s">
         <v>86</v>
@@ -38480,11 +38480,11 @@
       <c r="A299" s="11" t="n">
         <v>43261</v>
       </c>
-      <c r="B299" s="12" t="s">
+      <c r="B299" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C299" s="12" t="s">
         <v>605</v>
-      </c>
-      <c r="C299" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D299" s="10" t="s">
         <v>86</v>
@@ -38561,11 +38561,11 @@
       <c r="A300" s="11" t="n">
         <v>43554</v>
       </c>
-      <c r="B300" s="12" t="s">
+      <c r="B300" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C300" s="12" t="s">
         <v>605</v>
-      </c>
-      <c r="C300" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D300" s="10" t="s">
         <v>86</v>
@@ -38632,11 +38632,11 @@
       <c r="A301" s="11" t="n">
         <v>43750</v>
       </c>
-      <c r="B301" s="12" t="s">
+      <c r="B301" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C301" s="12" t="s">
         <v>605</v>
-      </c>
-      <c r="C301" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D301" s="10" t="s">
         <v>86</v>
@@ -38707,11 +38707,11 @@
       <c r="A302" s="11" t="n">
         <v>44485</v>
       </c>
-      <c r="B302" s="12" t="s">
+      <c r="B302" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C302" s="12" t="s">
         <v>605</v>
-      </c>
-      <c r="C302" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D302" s="10" t="s">
         <v>86</v>
@@ -38780,11 +38780,11 @@
       <c r="A303" s="11" t="n">
         <v>44856</v>
       </c>
-      <c r="B303" s="12" t="s">
+      <c r="B303" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C303" s="12" t="s">
         <v>605</v>
-      </c>
-      <c r="C303" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D303" s="10" t="s">
         <v>86</v>
@@ -38847,11 +38847,11 @@
       <c r="A304" s="11" t="n">
         <v>45353</v>
       </c>
-      <c r="B304" s="8" t="s">
+      <c r="B304" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C304" s="8" t="s">
         <v>605</v>
-      </c>
-      <c r="C304" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="D304" s="10" t="s">
         <v>86</v>
@@ -38927,10 +38927,10 @@
         <v>40692</v>
       </c>
       <c r="B305" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C305" s="8" t="s">
         <v>438</v>
-      </c>
-      <c r="C305" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D305" s="10" t="s">
         <v>86</v>
@@ -39006,10 +39006,10 @@
         <v>43218</v>
       </c>
       <c r="B306" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C306" s="8" t="s">
         <v>438</v>
-      </c>
-      <c r="C306" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D306" s="10" t="s">
         <v>52</v>
@@ -39089,10 +39089,10 @@
         <v>43569</v>
       </c>
       <c r="B307" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C307" s="8" t="s">
         <v>438</v>
-      </c>
-      <c r="C307" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D307" s="10" t="s">
         <v>52</v>
@@ -39168,10 +39168,10 @@
         <v>44724</v>
       </c>
       <c r="B308" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C308" s="8" t="s">
         <v>438</v>
-      </c>
-      <c r="C308" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D308" s="10" t="s">
         <v>52</v>
@@ -39243,10 +39243,10 @@
         <v>45031</v>
       </c>
       <c r="B309" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C309" s="8" t="s">
         <v>438</v>
-      </c>
-      <c r="C309" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D309" s="10" t="s">
         <v>52</v>
@@ -39326,10 +39326,10 @@
         <v>45416</v>
       </c>
       <c r="B310" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C310" s="8" t="s">
         <v>438</v>
-      </c>
-      <c r="C310" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D310" s="10" t="s">
         <v>52</v>
@@ -39406,11 +39406,11 @@
       <c r="A311" s="11" t="n">
         <v>44114</v>
       </c>
-      <c r="B311" s="8" t="s">
+      <c r="B311" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C311" s="8" t="s">
         <v>1865</v>
-      </c>
-      <c r="C311" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="D311" s="10" t="s">
         <v>113</v>
@@ -39465,11 +39465,11 @@
       <c r="A312" s="11" t="n">
         <v>44506</v>
       </c>
-      <c r="B312" s="8" t="s">
+      <c r="B312" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C312" s="8" t="s">
         <v>1865</v>
-      </c>
-      <c r="C312" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="D312" s="10" t="s">
         <v>113</v>
@@ -39526,11 +39526,11 @@
       <c r="A313" s="11" t="n">
         <v>44814</v>
       </c>
-      <c r="B313" s="8" t="s">
+      <c r="B313" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C313" s="8" t="s">
         <v>1865</v>
-      </c>
-      <c r="C313" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="D313" s="10" t="s">
         <v>113</v>
@@ -39580,10 +39580,10 @@
         <v>42070</v>
       </c>
       <c r="B314" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C314" s="8" t="s">
         <v>881</v>
-      </c>
-      <c r="C314" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D314" s="10" t="s">
         <v>52</v>
@@ -39658,11 +39658,11 @@
       <c r="A315" s="11" t="n">
         <v>43400</v>
       </c>
-      <c r="B315" s="8" t="s">
+      <c r="B315" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C315" s="8" t="s">
         <v>1872</v>
-      </c>
-      <c r="C315" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="D315" s="10" t="s">
         <v>113</v>
@@ -39725,11 +39725,11 @@
       <c r="A316" s="11" t="n">
         <v>43757</v>
       </c>
-      <c r="B316" s="8" t="s">
+      <c r="B316" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C316" s="8" t="s">
         <v>1872</v>
-      </c>
-      <c r="C316" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="D316" s="10" t="s">
         <v>113</v>
@@ -39785,10 +39785,10 @@
         <v>44821</v>
       </c>
       <c r="B317" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C317" s="8" t="s">
         <v>1872</v>
-      </c>
-      <c r="C317" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D317" s="10" t="s">
         <v>113</v>
@@ -39844,10 +39844,10 @@
         <v>45213</v>
       </c>
       <c r="B318" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C318" s="8" t="s">
         <v>1872</v>
-      </c>
-      <c r="C318" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D318" s="10" t="s">
         <v>113</v>
@@ -39880,11 +39880,11 @@
       <c r="A319" s="11" t="n">
         <v>45437</v>
       </c>
-      <c r="B319" s="8" t="s">
+      <c r="B319" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C319" s="8" t="s">
         <v>1872</v>
-      </c>
-      <c r="C319" s="10" t="s">
-        <v>112</v>
       </c>
       <c r="D319" s="10" t="s">
         <v>113</v>
@@ -39917,11 +39917,11 @@
       <c r="A320" s="11" t="n">
         <v>43617</v>
       </c>
-      <c r="B320" s="10" t="s">
+      <c r="B320" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C320" s="10" t="s">
         <v>1697</v>
-      </c>
-      <c r="C320" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D320" s="10" t="s">
         <v>86</v>
@@ -39995,10 +39995,10 @@
         <v>43757</v>
       </c>
       <c r="B321" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C321" s="8" t="s">
         <v>1697</v>
-      </c>
-      <c r="C321" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D321" s="10" t="s">
         <v>86</v>
@@ -40062,10 +40062,10 @@
         <v>44114</v>
       </c>
       <c r="B322" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C322" s="8" t="s">
         <v>1697</v>
-      </c>
-      <c r="C322" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D322" s="10" t="s">
         <v>86</v>
@@ -40143,10 +40143,10 @@
         <v>44457</v>
       </c>
       <c r="B323" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C323" s="8" t="s">
         <v>1697</v>
-      </c>
-      <c r="C323" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D323" s="10" t="s">
         <v>86</v>
@@ -40224,10 +40224,10 @@
         <v>45059</v>
       </c>
       <c r="B324" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C324" s="8" t="s">
         <v>1697</v>
-      </c>
-      <c r="C324" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D324" s="10" t="s">
         <v>86</v>
@@ -40261,10 +40261,10 @@
         <v>43589</v>
       </c>
       <c r="B325" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C325" s="8" t="s">
         <v>1716</v>
-      </c>
-      <c r="C325" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D325" s="10" t="s">
         <v>86</v>
@@ -40332,7 +40332,7 @@
         <v>43001</v>
       </c>
       <c r="B326" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C326" s="8" t="s">
         <v>198</v>
@@ -40472,7 +40472,7 @@
         <v>43022</v>
       </c>
       <c r="B327" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C327" s="8" t="s">
         <v>145</v>
@@ -40610,7 +40610,7 @@
         <v>43204</v>
       </c>
       <c r="B328" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C328" s="8" t="s">
         <v>219</v>
@@ -40744,7 +40744,7 @@
         <v>43225</v>
       </c>
       <c r="B329" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C329" s="8" t="s">
         <v>176</v>
@@ -40880,7 +40880,7 @@
         <v>43232</v>
       </c>
       <c r="B330" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C330" s="8" t="s">
         <v>215</v>
@@ -41006,10 +41006,10 @@
         <v>43365</v>
       </c>
       <c r="B331" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C331" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="C331" s="10" t="s">
-        <v>111</v>
       </c>
       <c r="D331" s="10" t="s">
         <v>113</v>
@@ -41122,7 +41122,7 @@
         <v>43379</v>
       </c>
       <c r="B332" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C332" s="8" t="s">
         <v>1980</v>
@@ -41230,7 +41230,7 @@
         <v>43393</v>
       </c>
       <c r="B333" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C333" s="8" t="s">
         <v>200</v>
@@ -41348,7 +41348,7 @@
         <v>43582</v>
       </c>
       <c r="B334" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C334" s="8" t="s">
         <v>181</v>
@@ -41462,7 +41462,7 @@
         <v>43589</v>
       </c>
       <c r="B335" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C335" s="8" t="s">
         <v>1872</v>
@@ -41576,7 +41576,7 @@
         <v>43743</v>
       </c>
       <c r="B336" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C336" s="8" t="s">
         <v>200</v>
@@ -41678,7 +41678,7 @@
         <v>44471</v>
       </c>
       <c r="B337" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C337" s="8" t="s">
         <v>2028</v>
@@ -41796,7 +41796,7 @@
         <v>44478</v>
       </c>
       <c r="B338" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C338" s="8" t="s">
         <v>1980</v>
@@ -41906,7 +41906,7 @@
         <v>44696</v>
       </c>
       <c r="B339" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C339" s="8" t="s">
         <v>181</v>
@@ -42008,10 +42008,10 @@
         <v>44702</v>
       </c>
       <c r="B340" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C340" s="8" t="s">
         <v>112</v>
-      </c>
-      <c r="C340" s="8" t="s">
-        <v>111</v>
       </c>
       <c r="D340" s="10" t="s">
         <v>113</v>
@@ -42132,7 +42132,7 @@
         <v>44723</v>
       </c>
       <c r="B341" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C341" s="8" t="s">
         <v>1865</v>
@@ -42254,7 +42254,7 @@
         <v>44842</v>
       </c>
       <c r="B342" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C342" s="8" t="s">
         <v>181</v>
@@ -42356,7 +42356,7 @@
         <v>45038</v>
       </c>
       <c r="B343" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C343" s="10" t="s">
         <v>215</v>
@@ -42456,7 +42456,7 @@
         <v>45045</v>
       </c>
       <c r="B344" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C344" s="8" t="s">
         <v>1865</v>
@@ -42568,7 +42568,7 @@
         <v>45052</v>
       </c>
       <c r="B345" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C345" s="8" t="s">
         <v>1872</v>
@@ -42628,7 +42628,7 @@
         <v>45080</v>
       </c>
       <c r="B346" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C346" s="8" t="s">
         <v>2028</v>
@@ -42728,7 +42728,7 @@
         <v>45200</v>
       </c>
       <c r="B347" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C347" s="8" t="s">
         <v>181</v>
@@ -42822,7 +42822,7 @@
         <v>45206</v>
       </c>
       <c r="B348" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C348" s="8" t="s">
         <v>2103</v>
@@ -42882,7 +42882,7 @@
         <v>45206</v>
       </c>
       <c r="B349" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C349" s="10" t="s">
         <v>215</v>
@@ -42988,7 +42988,7 @@
         <v>45227</v>
       </c>
       <c r="B350" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C350" s="8" t="s">
         <v>1872</v>
@@ -43048,7 +43048,7 @@
         <v>45367</v>
       </c>
       <c r="B351" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C351" s="10" t="s">
         <v>2103</v>
@@ -43152,7 +43152,7 @@
         <v>45388</v>
       </c>
       <c r="B352" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C352" s="10" t="s">
         <v>1872</v>
@@ -43254,7 +43254,7 @@
         <v>45402</v>
       </c>
       <c r="B353" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C353" s="10" t="s">
         <v>2103</v>
@@ -43314,7 +43314,7 @@
         <v>45416</v>
       </c>
       <c r="B354" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C354" s="10" t="s">
         <v>215</v>
@@ -43374,7 +43374,7 @@
         <v>45416</v>
       </c>
       <c r="B355" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C355" s="8" t="s">
         <v>2028</v>
@@ -43434,7 +43434,7 @@
         <v>45437</v>
       </c>
       <c r="B356" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C356" s="10" t="s">
         <v>2103</v>
@@ -43493,11 +43493,11 @@
       <c r="A357" s="11" t="n">
         <v>44087</v>
       </c>
-      <c r="B357" s="12" t="s">
+      <c r="B357" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C357" s="12" t="s">
         <v>2028</v>
-      </c>
-      <c r="C357" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D357" s="10" t="s">
         <v>113</v>
@@ -43560,11 +43560,11 @@
       <c r="A358" s="11" t="n">
         <v>44689</v>
       </c>
-      <c r="B358" s="12" t="s">
+      <c r="B358" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C358" s="12" t="s">
         <v>2028</v>
-      </c>
-      <c r="C358" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D358" s="10" t="s">
         <v>113</v>
@@ -43625,11 +43625,11 @@
       <c r="A359" s="11" t="n">
         <v>45200</v>
       </c>
-      <c r="B359" s="12" t="s">
+      <c r="B359" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C359" s="12" t="s">
         <v>2028</v>
-      </c>
-      <c r="C359" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D359" s="10" t="s">
         <v>113</v>
@@ -43678,11 +43678,11 @@
       <c r="A360" s="11" t="n">
         <v>45367</v>
       </c>
-      <c r="B360" s="12" t="s">
+      <c r="B360" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C360" s="12" t="s">
         <v>2028</v>
-      </c>
-      <c r="C360" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D360" s="10" t="s">
         <v>113</v>
@@ -43736,10 +43736,10 @@
         <v>41552</v>
       </c>
       <c r="B361" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C361" s="8" t="s">
         <v>692</v>
-      </c>
-      <c r="C361" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D361" s="9" t="s">
         <v>670</v>
@@ -43817,10 +43817,10 @@
         <v>42518</v>
       </c>
       <c r="B362" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C362" s="8" t="s">
         <v>692</v>
-      </c>
-      <c r="C362" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D362" s="10" t="s">
         <v>52</v>
@@ -43898,10 +43898,10 @@
         <v>42623</v>
       </c>
       <c r="B363" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C363" s="8" t="s">
         <v>692</v>
-      </c>
-      <c r="C363" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D363" s="10" t="s">
         <v>52</v>
@@ -43977,10 +43977,10 @@
         <v>43029</v>
       </c>
       <c r="B364" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C364" s="8" t="s">
         <v>692</v>
-      </c>
-      <c r="C364" s="8" t="s">
-        <v>28</v>
       </c>
       <c r="D364" s="10" t="s">
         <v>52</v>
@@ -44060,10 +44060,10 @@
         <v>42091</v>
       </c>
       <c r="B365" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C365" s="8" t="s">
         <v>1489</v>
-      </c>
-      <c r="C365" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D365" s="10" t="s">
         <v>86</v>
@@ -44127,10 +44127,10 @@
         <v>42511</v>
       </c>
       <c r="B366" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C366" s="8" t="s">
         <v>1489</v>
-      </c>
-      <c r="C366" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D366" s="10" t="s">
         <v>86</v>
@@ -44198,10 +44198,10 @@
         <v>42623</v>
       </c>
       <c r="B367" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C367" s="8" t="s">
         <v>1489</v>
-      </c>
-      <c r="C367" s="8" t="s">
-        <v>85</v>
       </c>
       <c r="D367" s="10" t="s">
         <v>278</v>
@@ -44271,10 +44271,10 @@
         <v>43407</v>
       </c>
       <c r="B368" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C368" s="8" t="s">
         <v>1980</v>
-      </c>
-      <c r="C368" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D368" s="10" t="s">
         <v>113</v>
@@ -44338,10 +44338,10 @@
         <v>43750</v>
       </c>
       <c r="B369" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C369" s="8" t="s">
         <v>1980</v>
-      </c>
-      <c r="C369" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D369" s="10" t="s">
         <v>113</v>
@@ -44375,10 +44375,10 @@
         <v>44674</v>
       </c>
       <c r="B370" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C370" s="8" t="s">
         <v>1980</v>
-      </c>
-      <c r="C370" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="D370" s="10" t="s">
         <v>113</v>

</xml_diff>